<commit_message>
DataAnalysis: created reports on lw2, lw3
</commit_message>
<xml_diff>
--- a/Data Analysis/LW3/Tips.xlsx
+++ b/Data Analysis/LW3/Tips.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\studies\Data Analysis\LW3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A1F6349-5EF6-4A19-90D1-5AFFC56F3150}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3162A8AE-A41B-4C0E-A0AB-B84ECDA75C65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9180" yWindow="630" windowWidth="21585" windowHeight="11370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23550" yWindow="3570" windowWidth="21585" windowHeight="11370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tip" sheetId="2" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1495" uniqueCount="390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1498" uniqueCount="393">
   <si>
     <t>total_bill</t>
   </si>
@@ -1219,6 +1219,15 @@
   </si>
   <si>
     <t xml:space="preserve">a </t>
+  </si>
+  <si>
+    <t>mr</t>
+  </si>
+  <si>
+    <t>tr</t>
+  </si>
+  <si>
+    <t>ttabl</t>
   </si>
 </sst>
 </file>
@@ -1302,9 +1311,6 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1336,6 +1342,9 @@
         <vertical/>
         <horizontal/>
       </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -1461,7 +1470,7 @@
     <tableColumn id="3" xr3:uid="{D65228F6-D035-42F8-B76B-78D3BB43C927}" name="(Xi - Xср)^2">
       <calculatedColumnFormula>N2^2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{24232717-326E-4EA2-806F-3128AC31F022}" name="Xi^2" dataDxfId="1">
+    <tableColumn id="4" xr3:uid="{24232717-326E-4EA2-806F-3128AC31F022}" name="Xi^2" dataDxfId="2">
       <calculatedColumnFormula>Таблица5[[#This Row],[Xi]]^2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1473,7 +1482,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{8E9A1CD7-5C9C-4154-A346-20475F25B4C1}" name="Таблица6" displayName="Таблица6" ref="R1:U245" totalsRowShown="0">
   <autoFilter ref="R1:U245" xr:uid="{8E9A1CD7-5C9C-4154-A346-20475F25B4C1}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{A561220A-76F3-4B59-95B4-A41A7302A1F5}" name="Yi" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{A561220A-76F3-4B59-95B4-A41A7302A1F5}" name="Yi" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{C3200CE1-9CBD-4404-AF43-03E3770F8443}" name="Yi - Yср">
       <calculatedColumnFormula>R2-$J$248</calculatedColumnFormula>
     </tableColumn>
@@ -1763,10 +1772,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{678195CA-1C98-4A8E-B9D8-A0695FB47393}">
-  <dimension ref="A1:W251"/>
+  <dimension ref="A1:W255"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K230" workbookViewId="0">
-      <selection activeCell="V248" sqref="V248"/>
+    <sheetView tabSelected="1" topLeftCell="J229" workbookViewId="0">
+      <selection activeCell="N257" sqref="N257"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17310,6 +17319,33 @@
       <c r="S251">
         <f>(S249 - J247 * J248) / (SQRT((S247 - J247^2) * (S248 - J248^2)))</f>
         <v>0.6757341092113649</v>
+      </c>
+    </row>
+    <row r="253" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R253" t="s">
+        <v>390</v>
+      </c>
+      <c r="S253">
+        <f>SQRT((1-S251^2)/(J249-2))</f>
+        <v>4.7385504184415429E-2</v>
+      </c>
+    </row>
+    <row r="254" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R254" t="s">
+        <v>391</v>
+      </c>
+      <c r="S254">
+        <f>S251/S253</f>
+        <v>14.260354951200592</v>
+      </c>
+    </row>
+    <row r="255" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R255" t="s">
+        <v>392</v>
+      </c>
+      <c r="S255">
+        <f>_xlfn.T.INV.2T(0.05,J249-1)</f>
+        <v>1.9697743954267517</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DataAnalysis: passed lw2, lw3
</commit_message>
<xml_diff>
--- a/Data Analysis/LW3/Tips.xlsx
+++ b/Data Analysis/LW3/Tips.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\studies\Data Analysis\LW3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\studies\Data Analysis\LW3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1E3A906-B850-41C5-8621-DDAF85BA0A85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED94A8DC-E037-4FA7-9505-180F9B86A001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tip" sheetId="2" r:id="rId1"/>
@@ -32,6 +32,9 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
+    </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -3230,7 +3233,6 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -3238,6 +3240,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -3832,16 +3835,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>577850</xdr:colOff>
-      <xdr:row>241</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>320675</xdr:colOff>
+      <xdr:row>251</xdr:row>
+      <xdr:rowOff>3175</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>488950</xdr:colOff>
-      <xdr:row>256</xdr:row>
-      <xdr:rowOff>107950</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>536575</xdr:colOff>
+      <xdr:row>265</xdr:row>
+      <xdr:rowOff>174625</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4229,28 +4232,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{678195CA-1C98-4A8E-B9D8-A0695FB47393}">
   <dimension ref="A1:Y255"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J212" workbookViewId="0">
-      <selection activeCell="W252" sqref="W252"/>
+    <sheetView tabSelected="1" topLeftCell="A187" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="AE229" sqref="AE229"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.7265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.7265625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.54296875" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.5703125" customWidth="1"/>
     <col min="15" max="15" width="13" customWidth="1"/>
-    <col min="18" max="18" width="9.26953125" customWidth="1"/>
-    <col min="19" max="19" width="12.7265625" customWidth="1"/>
+    <col min="18" max="18" width="9.28515625" customWidth="1"/>
+    <col min="19" max="19" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4306,7 +4309,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -4369,7 +4372,7 @@
         <v>17.159899999999997</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -4432,7 +4435,7 @@
         <v>17.164400000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -4495,7 +4498,7 @@
         <v>73.535000000000011</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -4558,7 +4561,7 @@
         <v>78.380799999999994</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -4621,7 +4624,7 @@
         <v>88.769899999999993</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -4684,7 +4687,7 @@
         <v>119.1159</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -4747,7 +4750,7 @@
         <v>17.54</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -4810,7 +4813,7 @@
         <v>83.865600000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -4873,7 +4876,7 @@
         <v>29.478399999999997</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -4936,7 +4939,7 @@
         <v>47.739399999999996</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -4999,7 +5002,7 @@
         <v>17.561699999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -5062,7 +5065,7 @@
         <v>176.29999999999998</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>36</v>
       </c>
@@ -5125,7 +5128,7 @@
         <v>24.209400000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>38</v>
       </c>
@@ -5188,7 +5191,7 @@
         <v>55.29</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>40</v>
       </c>
@@ -5251,7 +5254,7 @@
         <v>44.7866</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>42</v>
       </c>
@@ -5314,7 +5317,7 @@
         <v>84.593599999999995</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>44</v>
       </c>
@@ -5377,7 +5380,7 @@
         <v>17.251100000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>46</v>
       </c>
@@ -5440,7 +5443,7 @@
         <v>60.435899999999997</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>48</v>
       </c>
@@ -5503,7 +5506,7 @@
         <v>59.394999999999996</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>49</v>
       </c>
@@ -5566,7 +5569,7 @@
         <v>69.177499999999995</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>52</v>
       </c>
@@ -5629,7 +5632,7 @@
         <v>73.113600000000005</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>54</v>
       </c>
@@ -5692,7 +5695,7 @@
         <v>55.797499999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>56</v>
       </c>
@@ -5755,7 +5758,7 @@
         <v>35.167099999999998</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>58</v>
       </c>
@@ -5818,7 +5821,7 @@
         <v>298.80360000000002</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>60</v>
       </c>
@@ -5881,7 +5884,7 @@
         <v>63.027600000000007</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>62</v>
       </c>
@@ -5944,7 +5947,7 @@
         <v>41.675399999999996</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>64</v>
       </c>
@@ -6007,7 +6010,7 @@
         <v>26.74</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>65</v>
       </c>
@@ -6070,7 +6073,7 @@
         <v>25.38</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>66</v>
       </c>
@@ -6133,7 +6136,7 @@
         <v>93.309999999999988</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>68</v>
       </c>
@@ -6196,7 +6199,7 @@
         <v>58.949999999999996</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>69</v>
       </c>
@@ -6259,7 +6262,7 @@
         <v>13.8475</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>71</v>
       </c>
@@ -6322,7 +6325,7 @@
         <v>45.875</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>73</v>
       </c>
@@ -6385,7 +6388,7 @@
         <v>45.18</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>74</v>
       </c>
@@ -6448,7 +6451,7 @@
         <v>50.690500000000007</v>
       </c>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>76</v>
       </c>
@@ -6511,7 +6514,7 @@
         <v>58.140600000000006</v>
       </c>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>78</v>
       </c>
@@ -6574,7 +6577,7 @@
         <v>86.616</v>
       </c>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>80</v>
       </c>
@@ -6637,7 +6640,7 @@
         <v>32.619999999999997</v>
       </c>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>81</v>
       </c>
@@ -6700,7 +6703,7 @@
         <v>51.975099999999998</v>
       </c>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>83</v>
       </c>
@@ -6763,7 +6766,7 @@
         <v>43.173900000000003</v>
       </c>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>85</v>
       </c>
@@ -6826,7 +6829,7 @@
         <v>156.35</v>
       </c>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>86</v>
       </c>
@@ -6889,7 +6892,7 @@
         <v>35.929600000000001</v>
       </c>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>88</v>
       </c>
@@ -6952,7 +6955,7 @@
         <v>44.348400000000005</v>
       </c>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>90</v>
       </c>
@@ -7015,7 +7018,7 @@
         <v>42.656399999999998</v>
       </c>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>92</v>
       </c>
@@ -7078,7 +7081,7 @@
         <v>12.7776</v>
       </c>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>94</v>
       </c>
@@ -7141,7 +7144,7 @@
         <v>170.23999999999998</v>
       </c>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>96</v>
       </c>
@@ -7204,7 +7207,7 @@
         <v>54.87</v>
       </c>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>97</v>
       </c>
@@ -7267,7 +7270,7 @@
         <v>111.15</v>
       </c>
     </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>98</v>
       </c>
@@ -7330,7 +7333,7 @@
         <v>194.39999999999998</v>
       </c>
     </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>100</v>
       </c>
@@ -7393,7 +7396,7 @@
         <v>58.527499999999996</v>
       </c>
     </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>102</v>
       </c>
@@ -7456,7 +7459,7 @@
         <v>54.12</v>
       </c>
     </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>103</v>
       </c>
@@ -7519,7 +7522,7 @@
         <v>31.349999999999998</v>
       </c>
     </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>104</v>
       </c>
@@ -7582,7 +7585,7 @@
         <v>26.753999999999998</v>
       </c>
     </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>106</v>
       </c>
@@ -7645,7 +7648,7 @@
         <v>181.01200000000003</v>
       </c>
     </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>108</v>
       </c>
@@ -7708,7 +7711,7 @@
         <v>15.506399999999999</v>
       </c>
     </row>
-    <row r="56" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>110</v>
       </c>
@@ -7771,7 +7774,7 @@
         <v>110.93039999999999</v>
       </c>
     </row>
-    <row r="57" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>112</v>
       </c>
@@ -7834,7 +7837,7 @@
         <v>68.409899999999993</v>
       </c>
     </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>114</v>
       </c>
@@ -7897,7 +7900,7 @@
         <v>114.03</v>
       </c>
     </row>
-    <row r="59" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>116</v>
       </c>
@@ -7960,7 +7963,7 @@
         <v>39.615000000000002</v>
       </c>
     </row>
-    <row r="60" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>118</v>
       </c>
@@ -8023,7 +8026,7 @@
         <v>19.782399999999999</v>
       </c>
     </row>
-    <row r="61" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>120</v>
       </c>
@@ -8086,7 +8089,7 @@
         <v>324.85710000000006</v>
       </c>
     </row>
-    <row r="62" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>54</v>
       </c>
@@ -8149,7 +8152,7 @@
         <v>65.130899999999997</v>
       </c>
     </row>
-    <row r="63" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>123</v>
       </c>
@@ -8212,7 +8215,7 @@
         <v>27.62</v>
       </c>
     </row>
-    <row r="64" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>124</v>
       </c>
@@ -8275,7 +8278,7 @@
         <v>21.819599999999998</v>
       </c>
     </row>
-    <row r="65" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>96</v>
       </c>
@@ -8338,7 +8341,7 @@
         <v>68.770399999999995</v>
       </c>
     </row>
-    <row r="66" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>127</v>
       </c>
@@ -8401,7 +8404,7 @@
         <v>46.437600000000003</v>
       </c>
     </row>
-    <row r="67" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>129</v>
       </c>
@@ -8464,7 +8467,7 @@
         <v>63.251999999999995</v>
       </c>
     </row>
-    <row r="68" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>131</v>
       </c>
@@ -8527,7 +8530,7 @@
         <v>40.631500000000003</v>
       </c>
     </row>
-    <row r="69" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>82</v>
       </c>
@@ -8590,7 +8593,7 @@
         <v>3.07</v>
       </c>
     </row>
-    <row r="70" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>134</v>
       </c>
@@ -8653,7 +8656,7 @@
         <v>40.662299999999995</v>
       </c>
     </row>
-    <row r="71" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>136</v>
       </c>
@@ -8716,7 +8719,7 @@
         <v>31.370899999999999</v>
       </c>
     </row>
-    <row r="72" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>138</v>
       </c>
@@ -8779,7 +8782,7 @@
         <v>23.679399999999998</v>
       </c>
     </row>
-    <row r="73" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>140</v>
       </c>
@@ -8842,7 +8845,7 @@
         <v>51.21</v>
       </c>
     </row>
-    <row r="74" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>141</v>
       </c>
@@ -8905,7 +8908,7 @@
         <v>84.340400000000002</v>
       </c>
     </row>
-    <row r="75" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>143</v>
       </c>
@@ -8968,7 +8971,7 @@
         <v>126.4</v>
       </c>
     </row>
-    <row r="76" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>144</v>
       </c>
@@ -9031,7 +9034,7 @@
         <v>32.406000000000006</v>
       </c>
     </row>
-    <row r="77" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>146</v>
       </c>
@@ -9094,7 +9097,7 @@
         <v>13.137499999999999</v>
       </c>
     </row>
-    <row r="78" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>52</v>
       </c>
@@ -9157,7 +9160,7 @@
         <v>55.193600000000004</v>
       </c>
     </row>
-    <row r="79" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>149</v>
       </c>
@@ -9220,7 +9223,7 @@
         <v>108.8</v>
       </c>
     </row>
-    <row r="80" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>153</v>
       </c>
@@ -9283,7 +9286,7 @@
         <v>68.28</v>
       </c>
     </row>
-    <row r="81" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>154</v>
       </c>
@@ -9346,7 +9349,7 @@
         <v>46.855899999999998</v>
       </c>
     </row>
-    <row r="82" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>156</v>
       </c>
@@ -9409,7 +9412,7 @@
         <v>58.320000000000007</v>
       </c>
     </row>
-    <row r="83" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>157</v>
       </c>
@@ -9472,7 +9475,7 @@
         <v>56.643999999999998</v>
       </c>
     </row>
-    <row r="84" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>159</v>
       </c>
@@ -9535,7 +9538,7 @@
         <v>18.428100000000001</v>
       </c>
     </row>
-    <row r="85" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>161</v>
       </c>
@@ -9598,7 +9601,7 @@
         <v>163.4</v>
       </c>
     </row>
-    <row r="86" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>162</v>
       </c>
@@ -9661,7 +9664,7 @@
         <v>32.439399999999999</v>
       </c>
     </row>
-    <row r="87" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>164</v>
       </c>
@@ -9724,7 +9727,7 @@
         <v>180.0711</v>
       </c>
     </row>
-    <row r="88" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>166</v>
       </c>
@@ -9787,7 +9790,7 @@
         <v>26.06</v>
       </c>
     </row>
-    <row r="89" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>167</v>
       </c>
@@ -9850,7 +9853,7 @@
         <v>73.12</v>
       </c>
     </row>
-    <row r="90" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>168</v>
       </c>
@@ -9913,7 +9916,7 @@
         <v>144.55349999999999</v>
       </c>
     </row>
-    <row r="91" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>170</v>
       </c>
@@ -9976,7 +9979,7 @@
         <v>63.480000000000004</v>
       </c>
     </row>
-    <row r="92" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>171</v>
       </c>
@@ -10039,7 +10042,7 @@
         <v>86.91</v>
       </c>
     </row>
-    <row r="93" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>173</v>
       </c>
@@ -10102,7 +10105,7 @@
         <v>78.714999999999989</v>
       </c>
     </row>
-    <row r="94" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>174</v>
       </c>
@@ -10165,7 +10168,7 @@
         <v>5.75</v>
       </c>
     </row>
-    <row r="95" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>175</v>
       </c>
@@ -10228,7 +10231,7 @@
         <v>70.176000000000002</v>
       </c>
     </row>
-    <row r="96" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>176</v>
       </c>
@@ -10291,7 +10294,7 @@
         <v>73.9375</v>
       </c>
     </row>
-    <row r="97" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>178</v>
       </c>
@@ -10354,7 +10357,7 @@
         <v>190.00410000000002</v>
       </c>
     </row>
-    <row r="98" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>180</v>
       </c>
@@ -10417,7 +10420,7 @@
         <v>109.12</v>
       </c>
     </row>
-    <row r="99" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>181</v>
       </c>
@@ -10480,7 +10483,7 @@
         <v>18.044999999999998</v>
       </c>
     </row>
-    <row r="100" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>16</v>
       </c>
@@ -10543,7 +10546,7 @@
         <v>63.03</v>
       </c>
     </row>
-    <row r="101" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>182</v>
       </c>
@@ -10606,7 +10609,7 @@
         <v>18.690000000000001</v>
       </c>
     </row>
-    <row r="102" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>183</v>
       </c>
@@ -10669,7 +10672,7 @@
         <v>28.375</v>
       </c>
     </row>
-    <row r="103" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>184</v>
       </c>
@@ -10732,7 +10735,7 @@
         <v>46.14</v>
       </c>
     </row>
-    <row r="104" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>185</v>
       </c>
@@ -10795,7 +10798,7 @@
         <v>110.75</v>
       </c>
     </row>
-    <row r="105" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>186</v>
       </c>
@@ -10858,7 +10861,7 @@
         <v>78.021600000000007</v>
       </c>
     </row>
-    <row r="106" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>188</v>
       </c>
@@ -10921,7 +10924,7 @@
         <v>85.353600000000014</v>
       </c>
     </row>
-    <row r="107" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>189</v>
       </c>
@@ -10984,7 +10987,7 @@
         <v>25.190399999999997</v>
       </c>
     </row>
-    <row r="108" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>191</v>
       </c>
@@ -11047,7 +11050,7 @@
         <v>83.189399999999992</v>
       </c>
     </row>
-    <row r="109" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>193</v>
       </c>
@@ -11110,7 +11113,7 @@
         <v>108.15090000000001</v>
       </c>
     </row>
-    <row r="110" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>195</v>
       </c>
@@ -11173,7 +11176,7 @@
         <v>68.582399999999993</v>
       </c>
     </row>
-    <row r="111" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>196</v>
       </c>
@@ -11236,7 +11239,7 @@
         <v>57.24</v>
       </c>
     </row>
-    <row r="112" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>197</v>
       </c>
@@ -11299,7 +11302,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="113" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>198</v>
       </c>
@@ -11362,7 +11365,7 @@
         <v>7.25</v>
       </c>
     </row>
-    <row r="114" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>199</v>
       </c>
@@ -11425,7 +11428,7 @@
         <v>152.28</v>
       </c>
     </row>
-    <row r="115" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>200</v>
       </c>
@@ -11488,7 +11491,7 @@
         <v>61.072499999999991</v>
       </c>
     </row>
-    <row r="116" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>202</v>
       </c>
@@ -11551,7 +11554,7 @@
         <v>102.84</v>
       </c>
     </row>
-    <row r="117" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>203</v>
       </c>
@@ -11614,7 +11617,7 @@
         <v>60.584999999999994</v>
       </c>
     </row>
-    <row r="118" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>204</v>
       </c>
@@ -11677,7 +11680,7 @@
         <v>151.74510000000001</v>
       </c>
     </row>
-    <row r="119" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>206</v>
       </c>
@@ -11740,7 +11743,7 @@
         <v>15.975000000000001</v>
       </c>
     </row>
-    <row r="120" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>207</v>
       </c>
@@ -11803,7 +11806,7 @@
         <v>22.373999999999999</v>
       </c>
     </row>
-    <row r="121" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>209</v>
       </c>
@@ -11866,7 +11869,7 @@
         <v>70.313599999999994</v>
       </c>
     </row>
-    <row r="122" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>211</v>
       </c>
@@ -11929,7 +11932,7 @@
         <v>27.003899999999998</v>
       </c>
     </row>
-    <row r="123" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>212</v>
       </c>
@@ -11992,7 +11995,7 @@
         <v>22.5456</v>
       </c>
     </row>
-    <row r="124" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>214</v>
       </c>
@@ -12055,7 +12058,7 @@
         <v>35.65</v>
       </c>
     </row>
-    <row r="125" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>215</v>
       </c>
@@ -12118,7 +12121,7 @@
         <v>31.9</v>
       </c>
     </row>
-    <row r="126" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>216</v>
       </c>
@@ -12181,7 +12184,7 @@
         <v>31.4496</v>
       </c>
     </row>
-    <row r="127" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>218</v>
       </c>
@@ -12244,7 +12247,7 @@
         <v>125.16000000000001</v>
       </c>
     </row>
-    <row r="128" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>220</v>
       </c>
@@ -12307,7 +12310,7 @@
         <v>12.609599999999999</v>
       </c>
     </row>
-    <row r="129" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>222</v>
       </c>
@@ -12370,7 +12373,7 @@
         <v>29.04</v>
       </c>
     </row>
-    <row r="130" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>223</v>
       </c>
@@ -12433,7 +12436,7 @@
         <v>22.76</v>
       </c>
     </row>
-    <row r="131" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>224</v>
       </c>
@@ -12496,7 +12499,7 @@
         <v>49.747600000000006</v>
       </c>
     </row>
-    <row r="132" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>226</v>
       </c>
@@ -12559,7 +12562,7 @@
         <v>28.619999999999997</v>
       </c>
     </row>
-    <row r="133" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>227</v>
       </c>
@@ -12622,7 +12625,7 @@
         <v>57.364100000000001</v>
       </c>
     </row>
-    <row r="134" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>229</v>
       </c>
@@ -12685,7 +12688,7 @@
         <v>16.754999999999999</v>
       </c>
     </row>
-    <row r="135" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>230</v>
       </c>
@@ -12748,7 +12751,7 @@
         <v>24.52</v>
       </c>
     </row>
-    <row r="136" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>231</v>
       </c>
@@ -12811,7 +12814,7 @@
         <v>59.345000000000006</v>
       </c>
     </row>
-    <row r="137" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>232</v>
       </c>
@@ -12874,7 +12877,7 @@
         <v>10.637499999999999</v>
       </c>
     </row>
-    <row r="138" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>44</v>
       </c>
@@ -12937,7 +12940,7 @@
         <v>20.66</v>
       </c>
     </row>
-    <row r="139" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>233</v>
       </c>
@@ -13000,7 +13003,7 @@
         <v>28.3</v>
       </c>
     </row>
-    <row r="140" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>234</v>
       </c>
@@ -13063,7 +13066,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="141" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>235</v>
       </c>
@@ -13126,7 +13129,7 @@
         <v>36.19</v>
       </c>
     </row>
-    <row r="142" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>236</v>
       </c>
@@ -13189,7 +13192,7 @@
         <v>61.144999999999996</v>
       </c>
     </row>
-    <row r="143" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>237</v>
       </c>
@@ -13252,7 +13255,7 @@
         <v>229.80999999999997</v>
       </c>
     </row>
-    <row r="144" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>239</v>
       </c>
@@ -13315,7 +13318,7 @@
         <v>205.95</v>
       </c>
     </row>
-    <row r="145" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>240</v>
       </c>
@@ -13378,7 +13381,7 @@
         <v>135.25</v>
       </c>
     </row>
-    <row r="146" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>241</v>
       </c>
@@ -13441,7 +13444,7 @@
         <v>37.788999999999994</v>
       </c>
     </row>
-    <row r="147" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>243</v>
       </c>
@@ -13504,7 +13507,7 @@
         <v>12.524999999999999</v>
       </c>
     </row>
-    <row r="148" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>244</v>
       </c>
@@ -13567,7 +13570,7 @@
         <v>25.350400000000004</v>
       </c>
     </row>
-    <row r="149" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>246</v>
       </c>
@@ -13630,7 +13633,7 @@
         <v>19.348099999999999</v>
       </c>
     </row>
-    <row r="150" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>248</v>
       </c>
@@ -13693,7 +13696,7 @@
         <v>16.9194</v>
       </c>
     </row>
-    <row r="151" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>250</v>
       </c>
@@ -13756,7 +13759,7 @@
         <v>15.02</v>
       </c>
     </row>
-    <row r="152" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>251</v>
       </c>
@@ -13819,7 +13822,7 @@
         <v>35.174999999999997</v>
       </c>
     </row>
-    <row r="153" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>252</v>
       </c>
@@ -13882,7 +13885,7 @@
         <v>26.26</v>
       </c>
     </row>
-    <row r="154" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>253</v>
       </c>
@@ -13945,7 +13948,7 @@
         <v>47.292400000000008</v>
       </c>
     </row>
-    <row r="155" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>255</v>
       </c>
@@ -14008,7 +14011,7 @@
         <v>49.1</v>
       </c>
     </row>
-    <row r="156" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>256</v>
       </c>
@@ -14071,7 +14074,7 @@
         <v>39.54</v>
       </c>
     </row>
-    <row r="157" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>257</v>
       </c>
@@ -14134,7 +14137,7 @@
         <v>153.429</v>
       </c>
     </row>
-    <row r="158" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>259</v>
       </c>
@@ -14197,7 +14200,7 @@
         <v>240.85000000000002</v>
       </c>
     </row>
-    <row r="159" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>260</v>
       </c>
@@ -14260,7 +14263,7 @@
         <v>93.75</v>
       </c>
     </row>
-    <row r="160" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>262</v>
       </c>
@@ -14323,7 +14326,7 @@
         <v>34.947899999999997</v>
       </c>
     </row>
-    <row r="161" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>264</v>
       </c>
@@ -14386,7 +14389,7 @@
         <v>32.979999999999997</v>
       </c>
     </row>
-    <row r="162" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>265</v>
       </c>
@@ -14449,7 +14452,7 @@
         <v>75.25</v>
       </c>
     </row>
-    <row r="163" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>266</v>
       </c>
@@ -14512,7 +14515,7 @@
         <v>31.65</v>
       </c>
     </row>
-    <row r="164" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>267</v>
       </c>
@@ -14575,7 +14578,7 @@
         <v>32.42</v>
       </c>
     </row>
-    <row r="165" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>123</v>
       </c>
@@ -14638,7 +14641,7 @@
         <v>27.62</v>
       </c>
     </row>
-    <row r="166" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>268</v>
       </c>
@@ -14701,7 +14704,7 @@
         <v>52.53</v>
       </c>
     </row>
-    <row r="167" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>269</v>
       </c>
@@ -14764,7 +14767,7 @@
         <v>85.329599999999999</v>
       </c>
     </row>
-    <row r="168" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>270</v>
       </c>
@@ -14827,7 +14830,7 @@
         <v>46.502400000000009</v>
       </c>
     </row>
-    <row r="169" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>271</v>
       </c>
@@ -14890,7 +14893,7 @@
         <v>142.69499999999999</v>
       </c>
     </row>
-    <row r="170" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>273</v>
       </c>
@@ -14953,7 +14956,7 @@
         <v>17.049900000000001</v>
       </c>
     </row>
-    <row r="171" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>275</v>
       </c>
@@ -15016,7 +15019,7 @@
         <v>21.26</v>
       </c>
     </row>
-    <row r="172" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>276</v>
       </c>
@@ -15079,7 +15082,7 @@
         <v>508.1</v>
       </c>
     </row>
-    <row r="173" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>278</v>
       </c>
@@ -15142,7 +15145,7 @@
         <v>49.959600000000002</v>
       </c>
     </row>
-    <row r="174" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>198</v>
       </c>
@@ -15205,7 +15208,7 @@
         <v>37.337500000000006</v>
       </c>
     </row>
-    <row r="175" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>281</v>
       </c>
@@ -15268,7 +15271,7 @@
         <v>101.28300000000002</v>
       </c>
     </row>
-    <row r="176" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>282</v>
       </c>
@@ -15331,7 +15334,7 @@
         <v>67.28</v>
       </c>
     </row>
-    <row r="177" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>283</v>
       </c>
@@ -15394,7 +15397,7 @@
         <v>102.31899999999999</v>
       </c>
     </row>
-    <row r="178" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>285</v>
       </c>
@@ -15457,7 +15460,7 @@
         <v>35.78</v>
       </c>
     </row>
-    <row r="179" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>286</v>
       </c>
@@ -15520,7 +15523,7 @@
         <v>28.96</v>
       </c>
     </row>
-    <row r="180" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>287</v>
       </c>
@@ -15583,7 +15586,7 @@
         <v>38.4</v>
       </c>
     </row>
-    <row r="181" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>288</v>
       </c>
@@ -15646,7 +15649,7 @@
         <v>122.93650000000001</v>
       </c>
     </row>
-    <row r="182" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>290</v>
       </c>
@@ -15709,7 +15712,7 @@
         <v>127.512</v>
       </c>
     </row>
-    <row r="183" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>292</v>
       </c>
@@ -15772,7 +15775,7 @@
         <v>131.81450000000001</v>
       </c>
     </row>
-    <row r="184" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>294</v>
       </c>
@@ -15835,7 +15838,7 @@
         <v>158.72499999999999</v>
       </c>
     </row>
-    <row r="185" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>295</v>
       </c>
@@ -15898,7 +15901,7 @@
         <v>150.60500000000002</v>
       </c>
     </row>
-    <row r="186" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>297</v>
       </c>
@@ -15961,7 +15964,7 @@
         <v>121.64999999999999</v>
       </c>
     </row>
-    <row r="187" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>74</v>
       </c>
@@ -16024,7 +16027,7 @@
         <v>103.45</v>
       </c>
     </row>
-    <row r="188" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>298</v>
       </c>
@@ -16087,7 +16090,7 @@
         <v>73.149999999999991</v>
       </c>
     </row>
-    <row r="189" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>299</v>
       </c>
@@ -16150,7 +16153,7 @@
         <v>60.92</v>
       </c>
     </row>
-    <row r="190" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>300</v>
       </c>
@@ -16213,7 +16216,7 @@
         <v>63.524999999999991</v>
       </c>
     </row>
-    <row r="191" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>301</v>
       </c>
@@ -16276,7 +16279,7 @@
         <v>92.4</v>
       </c>
     </row>
-    <row r="192" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>302</v>
       </c>
@@ -16339,7 +16342,7 @@
         <v>23.535</v>
       </c>
     </row>
-    <row r="193" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>303</v>
       </c>
@@ -16402,7 +16405,7 @@
         <v>83.003900000000002</v>
       </c>
     </row>
-    <row r="194" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>305</v>
       </c>
@@ -16465,7 +16468,7 @@
         <v>72.806400000000011</v>
       </c>
     </row>
-    <row r="195" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>307</v>
       </c>
@@ -16528,7 +16531,7 @@
         <v>31.269600000000001</v>
       </c>
     </row>
-    <row r="196" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>309</v>
       </c>
@@ -16591,7 +16594,7 @@
         <v>66.319999999999993</v>
       </c>
     </row>
-    <row r="197" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>310</v>
       </c>
@@ -16654,7 +16657,7 @@
         <v>10.886399999999998</v>
       </c>
     </row>
-    <row r="198" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>13</v>
       </c>
@@ -16717,7 +16720,7 @@
         <v>20.68</v>
       </c>
     </row>
-    <row r="199" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>312</v>
       </c>
@@ -16780,7 +16783,7 @@
         <v>215.55</v>
       </c>
     </row>
-    <row r="200" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>313</v>
       </c>
@@ -16843,7 +16846,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="201" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>314</v>
       </c>
@@ -16906,7 +16909,7 @@
         <v>27.02</v>
       </c>
     </row>
-    <row r="202" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>315</v>
       </c>
@@ -16969,7 +16972,7 @@
         <v>74.84</v>
       </c>
     </row>
-    <row r="203" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>316</v>
       </c>
@@ -17032,7 +17035,7 @@
         <v>25.607399999999998</v>
       </c>
     </row>
-    <row r="204" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>313</v>
       </c>
@@ -17095,7 +17098,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="205" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>317</v>
       </c>
@@ -17158,7 +17161,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="206" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>318</v>
       </c>
@@ -17221,7 +17224,7 @@
         <v>82.12</v>
       </c>
     </row>
-    <row r="207" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>319</v>
       </c>
@@ -17284,7 +17287,7 @@
         <v>53.198099999999997</v>
       </c>
     </row>
-    <row r="208" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>320</v>
       </c>
@@ -17347,7 +17350,7 @@
         <v>90.671900000000008</v>
       </c>
     </row>
-    <row r="209" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>322</v>
       </c>
@@ -17410,7 +17413,7 @@
         <v>116.19</v>
       </c>
     </row>
-    <row r="210" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>323</v>
       </c>
@@ -17473,7 +17476,7 @@
         <v>49.268099999999997</v>
       </c>
     </row>
-    <row r="211" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>324</v>
       </c>
@@ -17536,7 +17539,7 @@
         <v>28.454799999999999</v>
       </c>
     </row>
-    <row r="212" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>325</v>
       </c>
@@ -17599,7 +17602,7 @@
         <v>60.12</v>
       </c>
     </row>
-    <row r="213" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>326</v>
       </c>
@@ -17662,7 +17665,7 @@
         <v>133.5924</v>
       </c>
     </row>
-    <row r="214" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>328</v>
       </c>
@@ -17725,7 +17728,7 @@
         <v>434.96999999999997</v>
       </c>
     </row>
-    <row r="215" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>330</v>
       </c>
@@ -17788,7 +17791,7 @@
         <v>33.174999999999997</v>
       </c>
     </row>
-    <row r="216" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>331</v>
       </c>
@@ -17851,7 +17854,7 @@
         <v>183.10500000000002</v>
       </c>
     </row>
-    <row r="217" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>332</v>
       </c>
@@ -17914,7 +17917,7 @@
         <v>14.190000000000001</v>
       </c>
     </row>
-    <row r="218" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>334</v>
       </c>
@@ -17977,7 +17980,7 @@
         <v>84.449999999999989</v>
       </c>
     </row>
-    <row r="219" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>335</v>
       </c>
@@ -18040,7 +18043,7 @@
         <v>17.384999999999998</v>
       </c>
     </row>
-    <row r="220" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>336</v>
       </c>
@@ -18103,7 +18106,7 @@
         <v>11.1456</v>
       </c>
     </row>
-    <row r="221" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>337</v>
       </c>
@@ -18166,7 +18169,7 @@
         <v>93.132599999999996</v>
       </c>
     </row>
-    <row r="222" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>339</v>
       </c>
@@ -18229,7 +18232,7 @@
         <v>26.752000000000002</v>
       </c>
     </row>
-    <row r="223" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>212</v>
       </c>
@@ -18292,7 +18295,7 @@
         <v>46.701599999999999</v>
       </c>
     </row>
-    <row r="224" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>340</v>
       </c>
@@ -18355,7 +18358,7 @@
         <v>16.473600000000001</v>
       </c>
     </row>
-    <row r="225" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>162</v>
       </c>
@@ -18418,7 +18421,7 @@
         <v>47.94</v>
       </c>
     </row>
-    <row r="226" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>212</v>
       </c>
@@ -18481,7 +18484,7 @@
         <v>21.203600000000002</v>
       </c>
     </row>
-    <row r="227" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>343</v>
       </c>
@@ -18544,7 +18547,7 @@
         <v>40.674999999999997</v>
       </c>
     </row>
-    <row r="228" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>344</v>
       </c>
@@ -18607,7 +18610,7 @@
         <v>20.18</v>
       </c>
     </row>
-    <row r="229" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>345</v>
       </c>
@@ -18670,7 +18673,7 @@
         <v>61.349999999999994</v>
       </c>
     </row>
-    <row r="230" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>346</v>
       </c>
@@ -18733,7 +18736,7 @@
         <v>36.121600000000001</v>
       </c>
     </row>
-    <row r="231" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>348</v>
       </c>
@@ -18796,7 +18799,7 @@
         <v>63.705600000000004</v>
       </c>
     </row>
-    <row r="232" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>350</v>
       </c>
@@ -18859,7 +18862,7 @@
         <v>48.02</v>
       </c>
     </row>
-    <row r="233" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>302</v>
       </c>
@@ -18922,7 +18925,7 @@
         <v>47.07</v>
       </c>
     </row>
-    <row r="234" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>351</v>
       </c>
@@ -18985,7 +18988,7 @@
         <v>39.357900000000001</v>
       </c>
     </row>
-    <row r="235" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>353</v>
       </c>
@@ -19048,7 +19051,7 @@
         <v>15.831899999999999</v>
       </c>
     </row>
-    <row r="236" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>355</v>
       </c>
@@ -19111,7 +19114,7 @@
         <v>46.589999999999996</v>
       </c>
     </row>
-    <row r="237" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>159</v>
       </c>
@@ -19174,7 +19177,7 @@
         <v>12.5875</v>
       </c>
     </row>
-    <row r="238" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>356</v>
       </c>
@@ -19237,7 +19240,7 @@
         <v>12.6</v>
       </c>
     </row>
-    <row r="239" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>357</v>
       </c>
@@ -19300,7 +19303,7 @@
         <v>38.411099999999998</v>
       </c>
     </row>
-    <row r="240" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>359</v>
       </c>
@@ -19363,7 +19366,7 @@
         <v>167.3261</v>
       </c>
     </row>
-    <row r="241" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>361</v>
       </c>
@@ -19426,7 +19429,7 @@
         <v>171.85759999999999</v>
       </c>
     </row>
-    <row r="242" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>363</v>
       </c>
@@ -19489,7 +19492,7 @@
         <v>54.36</v>
       </c>
     </row>
-    <row r="243" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>364</v>
       </c>
@@ -19552,7 +19555,7 @@
         <v>45.34</v>
       </c>
     </row>
-    <row r="244" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>365</v>
       </c>
@@ -19615,7 +19618,7 @@
         <v>31.185000000000002</v>
       </c>
     </row>
-    <row r="245" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>367</v>
       </c>
@@ -19678,7 +19681,7 @@
         <v>56.34</v>
       </c>
     </row>
-    <row r="247" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:25" x14ac:dyDescent="0.25">
       <c r="I247" t="s">
         <v>368</v>
       </c>
@@ -19722,7 +19725,7 @@
         <v>0.92026961355467307</v>
       </c>
     </row>
-    <row r="248" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:25" x14ac:dyDescent="0.25">
       <c r="I248" t="s">
         <v>369</v>
       </c>
@@ -19767,7 +19770,7 @@
         <v>7.2217406566158751</v>
       </c>
     </row>
-    <row r="249" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:25" x14ac:dyDescent="0.25">
       <c r="I249" t="s">
         <v>373</v>
       </c>
@@ -19782,7 +19785,7 @@
         <v>67.613159016393453</v>
       </c>
     </row>
-    <row r="251" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:25" x14ac:dyDescent="0.25">
       <c r="R251" t="s">
         <v>387</v>
       </c>
@@ -19791,7 +19794,7 @@
         <v>0.6757341092113649</v>
       </c>
     </row>
-    <row r="253" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:25" x14ac:dyDescent="0.25">
       <c r="R253" t="s">
         <v>390</v>
       </c>
@@ -19800,7 +19803,7 @@
         <v>4.7385504184415429E-2</v>
       </c>
     </row>
-    <row r="254" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:25" x14ac:dyDescent="0.25">
       <c r="R254" t="s">
         <v>391</v>
       </c>
@@ -19809,7 +19812,7 @@
         <v>14.260354951200592</v>
       </c>
     </row>
-    <row r="255" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:25" x14ac:dyDescent="0.25">
       <c r="R255" t="s">
         <v>392</v>
       </c>
@@ -19837,7 +19840,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>